<commit_message>
Example spreadsheet adom fix.
</commit_message>
<xml_diff>
--- a/roles/fortigate.ztp/files/spreadsheets/Ansible_ZTP_Local_Simple_Topology.xlsx
+++ b/roles/fortigate.ztp/files/spreadsheets/Ansible_ZTP_Local_Simple_Topology.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fortinet-my.sharepoint.com/personal/lweighall_fortinet-us_com/Documents/Ansible ZTP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1516" documentId="8_{76316668-8358-D540-AC45-49EE0DC0AD63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FAB6327F-7D99-B141-A112-2922B117B76C}"/>
+  <xr:revisionPtr revIDLastSave="1518" documentId="8_{76316668-8358-D540-AC45-49EE0DC0AD63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7E43944B-114A-9846-B139-D49FC6E59358}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="2180" windowWidth="38420" windowHeight="18760" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="359">
   <si>
     <t>VLAN ID</t>
   </si>
@@ -1065,9 +1065,6 @@
   </si>
   <si>
     <t>a-p</t>
-  </si>
-  <si>
-    <t>NA_64</t>
   </si>
   <si>
     <t>VOIP</t>
@@ -1871,10 +1868,10 @@
         <v>52</v>
       </c>
       <c r="H2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="J2" s="19" t="s">
         <v>238</v>
@@ -1910,16 +1907,16 @@
         <v>29</v>
       </c>
       <c r="C1" s="28" t="s">
+        <v>332</v>
+      </c>
+      <c r="D1" s="28" t="s">
         <v>333</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="E1" s="28" t="s">
         <v>334</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="F1" s="28" t="s">
         <v>335</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -1962,7 +1959,7 @@
         <v>131</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>133</v>
@@ -2013,10 +2010,10 @@
         <v>267</v>
       </c>
       <c r="W1" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="X1" s="9" t="s">
         <v>337</v>
-      </c>
-      <c r="X1" s="9" t="s">
-        <v>338</v>
       </c>
       <c r="Y1" s="9" t="s">
         <v>130</v>
@@ -3178,13 +3175,13 @@
         <v>221</v>
       </c>
       <c r="L1" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>340</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>341</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>130</v>
@@ -3401,13 +3398,13 @@
         <v>221</v>
       </c>
       <c r="K1" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>340</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>341</v>
       </c>
       <c r="N1" s="9" t="s">
         <v>130</v>
@@ -3594,13 +3591,13 @@
         <v>137</v>
       </c>
       <c r="F1" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>343</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -3857,10 +3854,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>347</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>33</v>
@@ -3871,13 +3868,13 @@
         <v>150</v>
       </c>
       <c r="B2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E2" t="s">
         <v>180</v>
@@ -3912,7 +3909,7 @@
         <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>135</v>
@@ -3923,13 +3920,13 @@
         <v>150</v>
       </c>
       <c r="B2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3937,13 +3934,13 @@
         <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -4349,8 +4346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4433,19 +4430,19 @@
         <v>101</v>
       </c>
       <c r="S1" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="U1" s="9" t="s">
         <v>328</v>
       </c>
-      <c r="T1" s="9" t="s">
-        <v>359</v>
-      </c>
-      <c r="U1" s="9" t="s">
-        <v>329</v>
-      </c>
       <c r="V1" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="W1" s="9" t="s">
         <v>356</v>
-      </c>
-      <c r="W1" s="9" t="s">
-        <v>357</v>
       </c>
       <c r="X1" s="9" t="s">
         <v>204</v>
@@ -4459,7 +4456,7 @@
         <v>145</v>
       </c>
       <c r="C2" t="s">
-        <v>322</v>
+        <v>145</v>
       </c>
       <c r="D2" t="s">
         <v>310</v>
@@ -4512,7 +4509,7 @@
         <v>145</v>
       </c>
       <c r="C3" t="s">
-        <v>322</v>
+        <v>145</v>
       </c>
       <c r="D3" t="s">
         <v>306</v>
@@ -4560,7 +4557,7 @@
         <v>15000</v>
       </c>
       <c r="S3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="X3" t="s">
         <v>182</v>
@@ -4601,7 +4598,7 @@
         <v>317</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>320</v>
@@ -4624,10 +4621,10 @@
         <v>321</v>
       </c>
       <c r="C2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D2" t="s">
         <v>325</v>
-      </c>
-      <c r="D2" t="s">
-        <v>326</v>
       </c>
       <c r="E2" t="s">
         <v>62</v>
@@ -4997,7 +4994,7 @@
         <v>223</v>
       </c>
       <c r="N2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -5134,7 +5131,7 @@
         <v>257</v>
       </c>
       <c r="G6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H6" t="s">
         <v>236</v>
@@ -6763,7 +6760,7 @@
         <v>240</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>241</v>
@@ -6772,13 +6769,13 @@
         <v>245</v>
       </c>
       <c r="J1" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>331</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>